<commit_message>
Created valid build by removing with sequences with a reverse orientation rep
</commit_message>
<xml_diff>
--- a/tabular/circo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/circo-ncbi-refseqs-side-data.xlsx
@@ -198,9 +198,6 @@
     <t>Mammal-2</t>
   </si>
   <si>
-    <t>sequence-ID</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -505,6 +502,9 @@
   </si>
   <si>
     <t>BtRp-CV-14</t>
+  </si>
+  <si>
+    <t>sequenceID</t>
   </si>
 </sst>
 </file>
@@ -1443,9 +1443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
@@ -1460,22 +1458,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="F1" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1495,18 +1493,18 @@
         <v>53</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -1520,7 +1518,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -1549,7 +1547,7 @@
         <v>53</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1569,7 +1567,7 @@
         <v>53</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1589,7 +1587,7 @@
         <v>53</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1609,7 +1607,7 @@
         <v>53</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1629,7 +1627,7 @@
         <v>53</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1649,7 +1647,7 @@
         <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1669,7 +1667,7 @@
         <v>54</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1689,7 +1687,7 @@
         <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1709,7 +1707,7 @@
         <v>55</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1729,7 +1727,7 @@
         <v>56</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1749,7 +1747,7 @@
         <v>52</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1769,7 +1767,7 @@
         <v>52</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1789,7 +1787,7 @@
         <v>52</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1809,7 +1807,7 @@
         <v>52</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1829,7 +1827,7 @@
         <v>57</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1849,475 +1847,475 @@
         <v>57</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="D21" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F21" s="13"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="D22" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F22" s="13"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>73</v>
-      </c>
       <c r="D23" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F23" s="13"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="C24" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>76</v>
-      </c>
       <c r="D24" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="C25" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>79</v>
-      </c>
       <c r="D25" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F25" s="13"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="C26" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="12" t="s">
-        <v>82</v>
-      </c>
       <c r="D26" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F26" s="13"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="12" t="s">
-        <v>88</v>
-      </c>
       <c r="D27" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F27" s="13"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="C28" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="12" t="s">
-        <v>92</v>
-      </c>
       <c r="E28" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="9" t="s">
-        <v>67</v>
-      </c>
       <c r="D29" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F29" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D30" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F30" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D31" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F31" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F33" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D34" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F34" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D35" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F35" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D36" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E36" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F36" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D37" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E37" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F37" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D38" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F38" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D39" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F39" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D40" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E40" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F40" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D41" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E41" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F41" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D42" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E42" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F42" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D43" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D45" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E45" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F45" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E46" s="11" t="s">
-        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged EVE data into this repository. Created a more complete build, ready for standard reporting
</commit_message>
<xml_diff>
--- a/tabular/circo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/circo-ncbi-refseqs-side-data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="183">
   <si>
     <t>PCV-1</t>
   </si>
@@ -375,9 +375,6 @@
     <t>NC_034977</t>
   </si>
   <si>
-    <t xml:space="preserve">bat </t>
-  </si>
-  <si>
     <t>NC_034547</t>
   </si>
   <si>
@@ -505,6 +502,75 @@
   </si>
   <si>
     <t>sequenceID</t>
+  </si>
+  <si>
+    <t>host range</t>
+  </si>
+  <si>
+    <t>Aves</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Columba livia</t>
+  </si>
+  <si>
+    <t>Metagenome</t>
+  </si>
+  <si>
+    <t>CyV-bat</t>
+  </si>
+  <si>
+    <t>DfCyV-4</t>
+  </si>
+  <si>
+    <t>DfCyV-A1</t>
+  </si>
+  <si>
+    <t>DuACyV-1/</t>
+  </si>
+  <si>
+    <t>BtCyV-GF-4c</t>
+  </si>
+  <si>
+    <t>BtCyV-POAII</t>
+  </si>
+  <si>
+    <t>BtCyV-POAVI</t>
+  </si>
+  <si>
+    <t>CyV-ZM36a</t>
+  </si>
+  <si>
+    <t>DfCyV5</t>
+  </si>
+  <si>
+    <t>FlCyV</t>
+  </si>
+  <si>
+    <t>CyV-VN</t>
+  </si>
+  <si>
+    <t>IE-CyV-IECSF08</t>
+  </si>
+  <si>
+    <t>HuCyV-GS140</t>
+  </si>
+  <si>
+    <t>HuCyV-VS5700009</t>
+  </si>
+  <si>
+    <t>DfCyV-2</t>
+  </si>
+  <si>
+    <t>FwCa-CyV-GS140</t>
+  </si>
+  <si>
+    <t>Rhinolophus pusillus</t>
+  </si>
+  <si>
+    <t>Bat sp.</t>
   </si>
 </sst>
 </file>
@@ -517,6 +583,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -645,7 +712,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="220">
+  <cellStyleXfs count="278">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -845,6 +912,64 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -887,7 +1012,7 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="220">
+  <cellStyles count="278">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1002,6 +1127,35 @@
     <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1107,6 +1261,35 @@
     <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1441,9 +1624,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G46" sqref="A1:G46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
@@ -1451,14 +1636,14 @@
     <col min="2" max="2" width="34.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="69.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="38.1640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="2"/>
+    <col min="5" max="6" width="18.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="38.1640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>58</v>
@@ -1472,11 +1657,14 @@
       <c r="E1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="F1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1492,19 +1680,22 @@
       <c r="E2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -1512,13 +1703,19 @@
       <c r="E3" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -1529,8 +1726,14 @@
       <c r="E4" s="9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="F4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1549,8 +1752,11 @@
       <c r="F5" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -1569,8 +1775,11 @@
       <c r="F6" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1589,8 +1798,11 @@
       <c r="F7" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1609,8 +1821,11 @@
       <c r="F8" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1629,8 +1844,11 @@
       <c r="F9" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1649,8 +1867,11 @@
       <c r="F10" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -1669,8 +1890,11 @@
       <c r="F11" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1689,8 +1913,11 @@
       <c r="F12" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1709,8 +1936,11 @@
       <c r="F13" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1729,8 +1959,11 @@
       <c r="F14" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1749,8 +1982,11 @@
       <c r="F15" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -1769,8 +2005,11 @@
       <c r="F16" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1789,8 +2028,11 @@
       <c r="F17" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1809,8 +2051,11 @@
       <c r="F18" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -1829,8 +2074,11 @@
       <c r="F19" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1849,8 +2097,11 @@
       <c r="F20" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="12" t="s">
         <v>82</v>
       </c>
@@ -1866,9 +2117,14 @@
       <c r="E21" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F21" s="13"/>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="F21" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>67</v>
       </c>
@@ -1884,9 +2140,14 @@
       <c r="E22" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="13"/>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="F22" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="12" t="s">
         <v>70</v>
       </c>
@@ -1902,9 +2163,14 @@
       <c r="E23" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="13"/>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="F23" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="12" t="s">
         <v>73</v>
       </c>
@@ -1920,9 +2186,14 @@
       <c r="E24" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="F24" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="12" t="s">
         <v>76</v>
       </c>
@@ -1938,9 +2209,14 @@
       <c r="E25" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="F25" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="12" t="s">
         <v>79</v>
       </c>
@@ -1956,9 +2232,14 @@
       <c r="E26" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="F26" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="12" t="s">
         <v>85</v>
       </c>
@@ -1974,9 +2255,14 @@
       <c r="E27" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="13"/>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="F27" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -1992,11 +2278,14 @@
       <c r="E28" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="13" t="s">
+      <c r="F28" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G28" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" s="9" t="s">
         <v>64</v>
       </c>
@@ -2012,15 +2301,20 @@
       <c r="E29" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G29" s="9" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B30" s="9"/>
+      <c r="B30" s="9" t="s">
+        <v>168</v>
+      </c>
       <c r="C30" s="9" t="s">
         <v>115</v>
       </c>
@@ -2030,17 +2324,22 @@
       <c r="E30" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>62</v>
@@ -2048,17 +2347,22 @@
       <c r="E31" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F31" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="F31" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" s="9"/>
+        <v>122</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>170</v>
+      </c>
       <c r="C32" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>62</v>
@@ -2066,17 +2370,22 @@
       <c r="E32" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>62</v>
@@ -2084,17 +2393,22 @@
       <c r="E33" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F33" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="F33" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="B34" s="9"/>
+        <v>126</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>172</v>
+      </c>
       <c r="C34" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>62</v>
@@ -2102,17 +2416,22 @@
       <c r="E34" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F34" s="9" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="F34" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B35" s="9"/>
+        <v>128</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>173</v>
+      </c>
       <c r="C35" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>62</v>
@@ -2120,17 +2439,22 @@
       <c r="E35" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:7">
       <c r="A36" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="B36" s="9"/>
+        <v>130</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>174</v>
+      </c>
       <c r="C36" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>62</v>
@@ -2138,17 +2462,22 @@
       <c r="E36" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F36" s="9" t="s">
+      <c r="F36" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:7">
       <c r="A37" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B37" s="9"/>
+        <v>135</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>175</v>
+      </c>
       <c r="C37" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>62</v>
@@ -2156,17 +2485,22 @@
       <c r="E37" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G37" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:7">
       <c r="A38" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="B38" s="9"/>
+        <v>137</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>176</v>
+      </c>
       <c r="C38" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>62</v>
@@ -2174,17 +2508,22 @@
       <c r="E38" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:7">
       <c r="A39" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B39" s="9"/>
+        <v>138</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>177</v>
+      </c>
       <c r="C39" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>62</v>
@@ -2192,17 +2531,22 @@
       <c r="E39" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B40" s="9"/>
+        <v>140</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>180</v>
+      </c>
       <c r="C40" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>62</v>
@@ -2210,17 +2554,22 @@
       <c r="E40" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G40" s="9" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:7">
       <c r="A41" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="B41" s="9"/>
+        <v>132</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>178</v>
+      </c>
       <c r="C41" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>62</v>
@@ -2228,17 +2577,22 @@
       <c r="E41" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="9" t="s">
+      <c r="F41" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G41" s="9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:7">
       <c r="A42" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="B42" s="9"/>
+        <v>142</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>179</v>
+      </c>
       <c r="C42" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>62</v>
@@ -2246,17 +2600,22 @@
       <c r="E42" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F42" s="9" t="s">
+      <c r="F42" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G42" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:7">
       <c r="A43" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>149</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>62</v>
@@ -2264,14 +2623,22 @@
       <c r="E43" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="9"/>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="F43" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>62</v>
@@ -2279,17 +2646,22 @@
       <c r="E44" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="F44" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B45" s="9"/>
+        <v>147</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>167</v>
+      </c>
       <c r="C45" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>62</v>
@@ -2297,25 +2669,34 @@
       <c r="E45" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G45" s="9" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:7">
       <c r="A46" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tidied up reference data
</commit_message>
<xml_diff>
--- a/tabular/circo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/circo-ncbi-refseqs-side-data.xlsx
@@ -1,34 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/DNAss/Circoviridae-GLUE/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA412E4-9230-9445-A929-FB07027065DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8260" yWindow="6520" windowWidth="30280" windowHeight="18820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="60" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="192">
   <si>
     <t>PCV-1</t>
   </si>
@@ -234,36 +228,24 @@
     <t>NC_025710</t>
   </si>
   <si>
-    <t>Circoviridae 5-LDMD-2013</t>
-  </si>
-  <si>
     <t>Circoviridae 5-LDMD-2014</t>
   </si>
   <si>
     <t>NC_025716</t>
   </si>
   <si>
-    <t>Circoviridae 11-LDMD-2013</t>
-  </si>
-  <si>
     <t>Circoviridae 11-LDMD-2014</t>
   </si>
   <si>
     <t>NC_025717</t>
   </si>
   <si>
-    <t>Circoviridae 13-LDMD-2013</t>
-  </si>
-  <si>
     <t>Circoviridae 13-LDMD-2014</t>
   </si>
   <si>
     <t>NC_025720</t>
   </si>
   <si>
-    <t>Circoviridae 16-LDMD-2013</t>
-  </si>
-  <si>
     <t>Circoviridae 16-LDMD-2014</t>
   </si>
   <si>
@@ -447,9 +429,6 @@
     <t>NC_023874</t>
   </si>
   <si>
-    <t>Florida woods cockroach-associated cyclovirus isolate GS140,</t>
-  </si>
-  <si>
     <t>NC_020206</t>
   </si>
   <si>
@@ -534,9 +513,6 @@
     <t>DfCyV-A1</t>
   </si>
   <si>
-    <t>DuACyV-1/</t>
-  </si>
-  <si>
     <t>BtCyV-GF-4c</t>
   </si>
   <si>
@@ -577,12 +553,57 @@
   </si>
   <si>
     <t>Bat sp.</t>
+  </si>
+  <si>
+    <t>KJ831064</t>
+  </si>
+  <si>
+    <t>KM382270</t>
+  </si>
+  <si>
+    <t>NC_025683</t>
+  </si>
+  <si>
+    <t>Po-Circo-like virus 41</t>
+  </si>
+  <si>
+    <t>Bat circovirus POA/2012/VI</t>
+  </si>
+  <si>
+    <t>Cyclovirus SL-108277</t>
+  </si>
+  <si>
+    <t>CyV-SL-108277</t>
+  </si>
+  <si>
+    <t>PoCv41</t>
+  </si>
+  <si>
+    <t>BtRp-CV-POA</t>
+  </si>
+  <si>
+    <t>Florida woods cockroach-associated cyclovirus isolate GS140</t>
+  </si>
+  <si>
+    <t>CV-5-LDMD-2013</t>
+  </si>
+  <si>
+    <t>CV-11-LDMD-2013</t>
+  </si>
+  <si>
+    <t>CV-13-LDMD-2013</t>
+  </si>
+  <si>
+    <t>CV-16-LDMD-2013</t>
+  </si>
+  <si>
+    <t>DuACyV-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -721,7 +742,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="278">
+  <cellStyleXfs count="316">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -921,6 +942,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1021,7 +1080,7 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="278">
+  <cellStyles count="316">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1165,6 +1224,25 @@
     <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1299,6 +1377,25 @@
     <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1635,27 +1732,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="A1:G46"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="34.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="69.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="63" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.1640625" style="2" customWidth="1"/>
     <col min="5" max="6" width="18.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="38.1640625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>58</v>
@@ -1670,13 +1767,13 @@
         <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
@@ -1693,21 +1790,21 @@
         <v>53</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -1716,18 +1813,18 @@
         <v>53</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -1739,13 +1836,13 @@
         <v>53</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>27</v>
       </c>
@@ -1762,13 +1859,13 @@
         <v>53</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -1785,13 +1882,13 @@
         <v>53</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>30</v>
       </c>
@@ -1808,13 +1905,13 @@
         <v>53</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -1831,13 +1928,13 @@
         <v>53</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -1854,13 +1951,13 @@
         <v>53</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1877,13 +1974,13 @@
         <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>33</v>
       </c>
@@ -1900,13 +1997,13 @@
         <v>54</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1923,13 +2020,13 @@
         <v>54</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -1946,13 +2043,13 @@
         <v>55</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -1969,13 +2066,13 @@
         <v>56</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1992,13 +2089,13 @@
         <v>52</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -2015,13 +2112,13 @@
         <v>52</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -2038,13 +2135,13 @@
         <v>52</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2061,13 +2158,13 @@
         <v>52</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
@@ -2084,13 +2181,13 @@
         <v>57</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2107,197 +2204,197 @@
         <v>57</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="D22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+      <c r="B23" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="D23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="B24" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C24" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="D24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B25" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="D25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="B26" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="C26" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" s="12" t="s">
+      <c r="D26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="B27" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="C28" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="D28" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>91</v>
-      </c>
       <c r="E28" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="9" t="s">
         <v>64</v>
       </c>
@@ -2314,21 +2411,21 @@
         <v>63</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>62</v>
@@ -2337,21 +2434,21 @@
         <v>63</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>62</v>
@@ -2360,21 +2457,21 @@
         <v>63</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D32" s="9" t="s">
         <v>62</v>
@@ -2383,21 +2480,21 @@
         <v>63</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>62</v>
@@ -2406,21 +2503,21 @@
         <v>63</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G33" s="9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="9" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>62</v>
@@ -2429,21 +2526,21 @@
         <v>63</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G34" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="9" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>128</v>
-      </c>
       <c r="B35" s="9" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>62</v>
@@ -2452,21 +2549,21 @@
         <v>63</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G35" s="9" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>62</v>
@@ -2475,21 +2572,21 @@
         <v>63</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>62</v>
@@ -2498,21 +2595,21 @@
         <v>63</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="9" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D38" s="9" t="s">
         <v>62</v>
@@ -2521,21 +2618,21 @@
         <v>63</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="9" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>62</v>
@@ -2544,21 +2641,21 @@
         <v>63</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="9" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>139</v>
+        <v>186</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>62</v>
@@ -2567,21 +2664,21 @@
         <v>63</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>62</v>
@@ -2590,21 +2687,21 @@
         <v>63</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D42" s="9" t="s">
         <v>62</v>
@@ -2613,21 +2710,21 @@
         <v>63</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>62</v>
@@ -2636,21 +2733,21 @@
         <v>63</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>62</v>
@@ -2659,21 +2756,21 @@
         <v>63</v>
       </c>
       <c r="F44" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="B45" s="9" t="s">
-        <v>167</v>
-      </c>
       <c r="C45" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>62</v>
@@ -2682,37 +2779,106 @@
         <v>63</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G46" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>181</v>
       </c>
+      <c r="D48" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G48" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="G49" s="12" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F186">
+  <sortState ref="A2:F186">
     <sortCondition ref="D2:D186"/>
     <sortCondition ref="E2:E186"/>
   </sortState>

</xml_diff>

<commit_message>
Corrected error in feature locations
</commit_message>
<xml_diff>
--- a/tabular/circo-ncbi-refseqs-side-data.xlsx
+++ b/tabular/circo-ncbi-refseqs-side-data.xlsx
@@ -576,9 +576,6 @@
     <t>CyV-SL-108277</t>
   </si>
   <si>
-    <t>PoCv41</t>
-  </si>
-  <si>
     <t>BtRp-CV-POA</t>
   </si>
   <si>
@@ -598,6 +595,9 @@
   </si>
   <si>
     <t>DuACyV-1</t>
+  </si>
+  <si>
+    <t>CvPo-41</t>
   </si>
 </sst>
 </file>
@@ -1735,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2238,7 +2238,7 @@
         <v>67</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>68</v>
@@ -2261,7 +2261,7 @@
         <v>69</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>70</v>
@@ -2284,7 +2284,7 @@
         <v>71</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>72</v>
@@ -2307,7 +2307,7 @@
         <v>73</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>74</v>
@@ -2422,7 +2422,7 @@
         <v>112</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>111</v>
@@ -2655,7 +2655,7 @@
         <v>174</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>62</v>
@@ -2836,7 +2836,7 @@
         <v>178</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>181</v>
@@ -2859,7 +2859,7 @@
         <v>179</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>180</v>

</xml_diff>